<commit_message>
Visit List Test Case Updated
</commit_message>
<xml_diff>
--- a/OrionProjectsWorkingCopy/DataFiles/Dev/Platform.xlsx
+++ b/OrionProjectsWorkingCopy/DataFiles/Dev/Platform.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rv042687/git/SeleniumV21Dec2016/OrionProjectsWorkingCopy/DataFiles/Dev/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rv042687/git/NewWorkingCopyJan6/OrionProjectsWorkingCopy/DataFiles/Dev/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PatientSearch" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="87">
   <si>
     <t>ORN_VR_PatientSearch</t>
   </si>
@@ -226,12 +226,78 @@
   </si>
   <si>
     <t>Recurring</t>
+  </si>
+  <si>
+    <t>Antonelli, Michael</t>
+  </si>
+  <si>
+    <t>Observation</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>Office Visit</t>
+  </si>
+  <si>
+    <t>Inpatient</t>
+  </si>
+  <si>
+    <t>Preadmit</t>
+  </si>
+  <si>
+    <t>PrvEnc2_DiscDate</t>
+  </si>
+  <si>
+    <t>PrvEnc2_Service</t>
+  </si>
+  <si>
+    <t>PrvEnc2_Location</t>
+  </si>
+  <si>
+    <t>PrvEnc2_RoomBed</t>
+  </si>
+  <si>
+    <t>PrvEnc2_FIN</t>
+  </si>
+  <si>
+    <t>PrvEnc2_Status</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Baseline East</t>
+  </si>
+  <si>
+    <t>FutEnc5_DiscDate</t>
+  </si>
+  <si>
+    <t>FutEnc5_Service</t>
+  </si>
+  <si>
+    <t>FutEnc5_Location</t>
+  </si>
+  <si>
+    <t>FutEnc5_RoomBed</t>
+  </si>
+  <si>
+    <t>FutEnc5_FIN</t>
+  </si>
+  <si>
+    <t>FutEnc5_Status</t>
+  </si>
+  <si>
+    <t>BU-BSC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="mmm\ d\,\ yyyy\ h:mm\ AM/PM;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -249,7 +315,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -274,6 +340,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -287,7 +359,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -307,6 +379,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -705,10 +789,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AT2"/>
+  <dimension ref="A1:BF2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AE5" sqref="AE5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -721,37 +805,42 @@
     <col min="6" max="6" width="14.33203125" customWidth="1"/>
     <col min="7" max="8" width="22.1640625" customWidth="1"/>
     <col min="9" max="9" width="24.5" customWidth="1"/>
-    <col min="10" max="10" width="44.33203125" customWidth="1"/>
+    <col min="10" max="10" width="24" style="11" customWidth="1"/>
     <col min="11" max="11" width="21.83203125" customWidth="1"/>
     <col min="12" max="12" width="12.5" customWidth="1"/>
     <col min="13" max="13" width="14.83203125" customWidth="1"/>
-    <col min="14" max="14" width="19.5" customWidth="1"/>
+    <col min="14" max="14" width="19.5" style="11" customWidth="1"/>
     <col min="15" max="15" width="15" customWidth="1"/>
     <col min="16" max="16" width="14.83203125" customWidth="1"/>
-    <col min="17" max="17" width="17.6640625" customWidth="1"/>
-    <col min="18" max="18" width="15.33203125" customWidth="1"/>
-    <col min="19" max="19" width="17.1640625" customWidth="1"/>
-    <col min="20" max="20" width="16.83203125" customWidth="1"/>
-    <col min="21" max="21" width="18.6640625" customWidth="1"/>
-    <col min="22" max="22" width="14.6640625" customWidth="1"/>
-    <col min="23" max="23" width="17.5" customWidth="1"/>
-    <col min="24" max="24" width="15.5" customWidth="1"/>
-    <col min="25" max="25" width="18.1640625" customWidth="1"/>
-    <col min="26" max="26" width="15.33203125" customWidth="1"/>
-    <col min="27" max="27" width="14" customWidth="1"/>
-    <col min="28" max="28" width="15.6640625" customWidth="1"/>
-    <col min="29" max="29" width="15.33203125" customWidth="1"/>
-    <col min="30" max="30" width="17.1640625" customWidth="1"/>
-    <col min="31" max="31" width="19.1640625" customWidth="1"/>
-    <col min="32" max="32" width="22.5" customWidth="1"/>
-    <col min="33" max="33" width="17.33203125" customWidth="1"/>
-    <col min="34" max="34" width="15.83203125" customWidth="1"/>
+    <col min="17" max="23" width="17.6640625" customWidth="1"/>
+    <col min="24" max="24" width="21" style="11" customWidth="1"/>
+    <col min="25" max="25" width="24" customWidth="1"/>
+    <col min="26" max="26" width="16.83203125" customWidth="1"/>
+    <col min="27" max="27" width="18.6640625" customWidth="1"/>
+    <col min="28" max="28" width="21.33203125" style="11" customWidth="1"/>
+    <col min="29" max="29" width="17.5" customWidth="1"/>
+    <col min="30" max="30" width="15.5" customWidth="1"/>
+    <col min="31" max="31" width="18.1640625" customWidth="1"/>
+    <col min="32" max="32" width="23.33203125" style="11" customWidth="1"/>
+    <col min="33" max="33" width="14" customWidth="1"/>
+    <col min="34" max="34" width="15.6640625" customWidth="1"/>
     <col min="35" max="35" width="15.33203125" customWidth="1"/>
-    <col min="36" max="36" width="16.5" customWidth="1"/>
-    <col min="37" max="37" width="19" customWidth="1"/>
+    <col min="36" max="36" width="16.33203125" customWidth="1"/>
+    <col min="37" max="37" width="15.33203125" customWidth="1"/>
+    <col min="38" max="38" width="17.1640625" customWidth="1"/>
+    <col min="39" max="39" width="17.6640625" customWidth="1"/>
+    <col min="40" max="41" width="15.33203125" customWidth="1"/>
+    <col min="42" max="42" width="19.83203125" style="14" customWidth="1"/>
+    <col min="43" max="43" width="19.1640625" customWidth="1"/>
+    <col min="44" max="44" width="22.5" customWidth="1"/>
+    <col min="45" max="45" width="17.33203125" customWidth="1"/>
+    <col min="46" max="46" width="22.1640625" style="11" customWidth="1"/>
+    <col min="47" max="47" width="15.33203125" customWidth="1"/>
+    <col min="48" max="48" width="16.5" customWidth="1"/>
+    <col min="49" max="49" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:58" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
@@ -779,7 +868,7 @@
       <c r="I1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="10" t="s">
         <v>36</v>
       </c>
       <c r="K1" s="5" t="s">
@@ -791,7 +880,7 @@
       <c r="M1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="12" t="s">
         <v>40</v>
       </c>
       <c r="O1" s="4" t="s">
@@ -803,73 +892,109 @@
       <c r="Q1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="R1" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="X1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="Z1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="AA1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="AB1" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="AF1" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AG1" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AH1" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AI1" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AJ1" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="AK1" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="AL1" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM1" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN1" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="AO1" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="AP1" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AR1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AS1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="AH1" s="5" t="s">
+      <c r="AT1" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="AI1" s="5" t="s">
+      <c r="AU1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="AJ1" s="5" t="s">
+      <c r="AV1" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="AK1" s="5" t="s">
+      <c r="AW1" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="AP1" s="6"/>
-      <c r="AQ1" s="6"/>
-      <c r="AR1" s="6"/>
-      <c r="AS1" s="6"/>
-      <c r="AT1" s="6"/>
+      <c r="BB1" s="6"/>
+      <c r="BC1" s="6"/>
+      <c r="BD1" s="6"/>
+      <c r="BE1" s="6"/>
+      <c r="BF1" s="6"/>
     </row>
-    <row r="2" spans="1:46" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:58" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>25</v>
       </c>
@@ -897,15 +1022,125 @@
       <c r="I2" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="7"/>
-      <c r="N2" s="7">
+      <c r="J2" s="9">
+        <v>42402.705555555556</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="N2" s="9">
         <v>42503.664583333331</v>
+      </c>
+      <c r="O2" s="15" t="s">
+        <v>68</v>
       </c>
       <c r="P2" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="S2" s="8" t="s">
+      <c r="Q2" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="R2" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="S2" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="T2" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="U2" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="V2" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="W2" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="X2" s="9">
+        <v>42570.208333333336</v>
+      </c>
+      <c r="Y2" s="8" t="s">
         <v>64</v>
+      </c>
+      <c r="Z2" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA2" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB2" s="9">
+        <v>42762.899305555555</v>
+      </c>
+      <c r="AC2" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD2" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE2" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF2" s="9">
+        <v>45658.25</v>
+      </c>
+      <c r="AG2" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="AH2" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI2" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ2" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="AK2" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL2" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="AM2" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN2" s="15">
+        <v>20002119</v>
+      </c>
+      <c r="AO2" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="AP2" s="9">
+        <v>47005.208333333336</v>
+      </c>
+      <c r="AQ2" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="AR2" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="AS2" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="AT2" s="9">
+        <v>42129.660416666666</v>
+      </c>
+      <c r="AU2" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="AV2" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AW2" s="15" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>